<commit_message>
Published state of ETDataset for deploy April 2022
</commit_message>
<xml_diff>
--- a/analyses/4a_metal_industry_analysis.xlsx
+++ b/analyses/4a_metal_industry_analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michieldenhaan/Code/etdataset/analyses/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathijsbijkerk/Projects/etdataset/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B16BCA-39F7-0B4C-8AC7-572E32DA7D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{521C3FF9-F887-9945-8A02-CE626E5BF814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="27660" windowHeight="17500" tabRatio="835" firstSheet="29" activeTab="31" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27660" windowHeight="17500" tabRatio="835" firstSheet="13" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="34" r:id="rId1"/>
@@ -261,7 +261,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1187" uniqueCount="655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1183" uniqueCount="651">
   <si>
     <t>Changelog</t>
   </si>
@@ -1805,9 +1805,6 @@
     <t>output.loss</t>
   </si>
   <si>
-    <t>energy_cokesoven_transformation_coal.converter</t>
-  </si>
-  <si>
     <t>industry_aluminium_electrolysis_current_electricity.converter</t>
   </si>
   <si>
@@ -2219,16 +2216,7 @@
     <t>Final demand conversion of steel production by scrap and HBI with EAF</t>
   </si>
   <si>
-    <t>energy_blastfurnace_own_use.converter</t>
-  </si>
-  <si>
-    <t>energy_cokesoven_own_use.converter</t>
-  </si>
-  <si>
     <t>industry_steel_scrap_hbi_eaf_efficiency</t>
-  </si>
-  <si>
-    <t>energy_blastfurnace_transformation_cokes.converter</t>
   </si>
   <si>
     <t>energy_blastfurnace_transformation_cokes_efficiency</t>
@@ -13014,6 +13002,7 @@
     <sheetNames>
       <sheetName val="Cover sheet"/>
       <sheetName val="Dashboard"/>
+      <sheetName val="analysis_manager"/>
     </sheetNames>
     <definedNames>
       <definedName name="export_data_button"/>
@@ -13023,6 +13012,7 @@
     <sheetDataSet>
       <sheetData sheetId="0"/>
       <sheetData sheetId="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -13378,7 +13368,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D4" s="5"/>
     </row>
@@ -13427,7 +13417,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D9" s="7"/>
     </row>
@@ -14548,7 +14538,7 @@
   <sheetData>
     <row r="2" spans="2:5" ht="21" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
@@ -14568,7 +14558,7 @@
     <row r="6" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="2:5" s="225" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B7" s="223" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C7" s="224"/>
       <c r="D7" s="484"/>
@@ -14875,7 +14865,7 @@
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B37" s="471" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="343"/>
@@ -14944,7 +14934,7 @@
   <sheetData>
     <row r="2" spans="2:5" ht="21" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
@@ -15001,7 +14991,7 @@
     <row r="11" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B11" s="472"/>
       <c r="C11" s="159" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D11" s="341">
         <f>'Steel and alu demand'!N12</f>
@@ -15015,7 +15005,7 @@
     <row r="12" spans="2:5" ht="34" x14ac:dyDescent="0.2">
       <c r="B12" s="472"/>
       <c r="C12" s="159" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D12" s="341">
         <f>'Steel and alu demand'!N13</f>
@@ -15029,7 +15019,7 @@
     <row r="13" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B13" s="472"/>
       <c r="C13" s="671" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D13" s="341">
         <f>'Steel and alu demand'!N14</f>
@@ -15043,7 +15033,7 @@
     <row r="14" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B14" s="472"/>
       <c r="C14" s="671" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="D14" s="341">
         <f>'Steel and alu demand'!N15</f>
@@ -15057,7 +15047,7 @@
     <row r="15" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B15" s="472"/>
       <c r="C15" s="671" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D15" s="341">
         <f>'Steel and alu demand'!N16</f>
@@ -15071,7 +15061,7 @@
     <row r="16" spans="2:5" ht="34" x14ac:dyDescent="0.2">
       <c r="B16" s="472"/>
       <c r="C16" s="159" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="D16" s="341">
         <v>0</v>
@@ -15084,7 +15074,7 @@
     <row r="17" spans="2:5" ht="34" x14ac:dyDescent="0.2">
       <c r="B17" s="472"/>
       <c r="C17" s="159" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D17" s="341">
         <v>0</v>
@@ -15097,7 +15087,7 @@
     <row r="18" spans="2:5" ht="34" x14ac:dyDescent="0.2">
       <c r="B18" s="472"/>
       <c r="C18" s="671" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="D18" s="341">
         <v>0</v>
@@ -15110,7 +15100,7 @@
     <row r="19" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B19" s="472"/>
       <c r="C19" s="671" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="D19" s="341">
         <v>0</v>
@@ -15137,7 +15127,7 @@
     <row r="22" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B22" s="472"/>
       <c r="C22" s="159" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D22" s="341">
         <f>'Steel and alu demand'!G12</f>
@@ -15151,7 +15141,7 @@
     <row r="23" spans="2:5" ht="34" x14ac:dyDescent="0.2">
       <c r="B23" s="472"/>
       <c r="C23" s="159" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D23" s="341">
         <f>'Steel and alu demand'!G13</f>
@@ -15165,7 +15155,7 @@
     <row r="24" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B24" s="472"/>
       <c r="C24" s="671" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D24" s="341">
         <f>'Steel and alu demand'!G14</f>
@@ -15179,7 +15169,7 @@
     <row r="25" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B25" s="472"/>
       <c r="C25" s="671" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="D25" s="341">
         <f>'Steel and alu demand'!G15</f>
@@ -15193,7 +15183,7 @@
     <row r="26" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B26" s="472"/>
       <c r="C26" s="671" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D26" s="341">
         <f>'Steel and alu demand'!G16</f>
@@ -15221,7 +15211,7 @@
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B29" s="472"/>
       <c r="C29" s="15" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D29" s="341">
         <f>'Steel and alu demand'!I12</f>
@@ -15249,7 +15239,7 @@
     <row r="32" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B32" s="472"/>
       <c r="C32" s="15" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D32" s="341">
         <f>'Steel and alu demand'!H12</f>
@@ -15277,7 +15267,7 @@
     <row r="35" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B35" s="472"/>
       <c r="C35" s="159" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D35" s="341">
         <f>'Steel and alu demand'!J12</f>
@@ -15291,7 +15281,7 @@
     <row r="36" spans="2:5" ht="34" x14ac:dyDescent="0.2">
       <c r="B36" s="472"/>
       <c r="C36" s="159" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D36" s="341">
         <f>'Steel and alu demand'!J13</f>
@@ -15305,7 +15295,7 @@
     <row r="37" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B37" s="472"/>
       <c r="C37" s="671" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D37" s="341">
         <f>'Steel and alu demand'!J14</f>
@@ -15319,7 +15309,7 @@
     <row r="38" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B38" s="472"/>
       <c r="C38" s="671" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="D38" s="341">
         <f>'Steel and alu demand'!J15</f>
@@ -15333,7 +15323,7 @@
     <row r="39" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B39" s="472"/>
       <c r="C39" s="671" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D39" s="341">
         <f>'Steel and alu demand'!J16</f>
@@ -15361,7 +15351,7 @@
     <row r="42" spans="2:5" ht="34" x14ac:dyDescent="0.2">
       <c r="B42" s="472"/>
       <c r="C42" s="159" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D42" s="341">
         <f>'Steel and alu demand'!L10</f>
@@ -15389,7 +15379,7 @@
     <row r="45" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B45" s="472"/>
       <c r="C45" s="159" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D45" s="341">
         <f>'Steel and alu demand'!K12</f>
@@ -15417,7 +15407,7 @@
     <row r="48" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B48" s="472"/>
       <c r="C48" s="159" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D48" s="341">
         <f>'Steel and alu demand'!M12</f>
@@ -15431,7 +15421,7 @@
     <row r="49" spans="2:5" ht="34" x14ac:dyDescent="0.2">
       <c r="B49" s="472"/>
       <c r="C49" s="159" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D49" s="341">
         <f>'Steel and alu demand'!M13</f>
@@ -15482,7 +15472,7 @@
   <sheetData>
     <row r="2" spans="2:5" ht="21" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
@@ -15689,8 +15679,8 @@
   </sheetPr>
   <dimension ref="B2:E26"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15705,7 +15695,7 @@
   <sheetData>
     <row r="2" spans="2:5" ht="21" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
@@ -15718,7 +15708,7 @@
     </row>
     <row r="5" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="708" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C5" s="709"/>
       <c r="D5" s="709"/>
@@ -15727,7 +15717,7 @@
     <row r="6" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" s="223" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C7" s="153"/>
       <c r="D7" s="484"/>
@@ -15743,7 +15733,7 @@
       <c r="B9" s="480"/>
       <c r="C9" s="487"/>
       <c r="D9" s="635" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E9" s="636" t="s">
         <v>391</v>
@@ -15751,7 +15741,7 @@
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B10" s="471" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C10" s="637"/>
       <c r="D10" s="638"/>
@@ -15800,7 +15790,7 @@
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B15" s="471" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C15" s="645"/>
       <c r="D15" s="646"/>
@@ -15817,7 +15807,7 @@
     <row r="17" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B17" s="156"/>
       <c r="C17" s="641" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D17" s="642">
         <f>-'Fuel aggregation'!G11</f>
@@ -15831,7 +15821,7 @@
     <row r="18" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B18" s="156"/>
       <c r="C18" s="641" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D18" s="642">
         <f>-'Fuel aggregation'!G12</f>
@@ -15853,10 +15843,10 @@
     <row r="20" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B20" s="27"/>
       <c r="C20" s="641" t="s">
-        <v>25</v>
+        <v>143</v>
       </c>
       <c r="D20" s="649">
-        <f>'Fuel aggregation'!G22</f>
+        <f>'Fuel aggregation'!G23</f>
         <v>0</v>
       </c>
       <c r="E20" s="647">
@@ -16061,7 +16051,7 @@
     <row r="12" spans="2:15" s="137" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B12" s="495"/>
       <c r="C12" s="493" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D12" s="109">
         <f>'Steel and alu prod'!E11</f>
@@ -16109,7 +16099,7 @@
     <row r="13" spans="2:15" s="137" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B13" s="495"/>
       <c r="C13" s="493" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D13" s="109">
         <f>'Steel and alu prod'!E12</f>
@@ -16130,7 +16120,7 @@
     <row r="14" spans="2:15" s="137" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B14" s="495"/>
       <c r="C14" s="493" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D14" s="109">
         <f>'Steel and alu prod'!E13</f>
@@ -16166,7 +16156,7 @@
     <row r="15" spans="2:15" s="137" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B15" s="495"/>
       <c r="C15" s="493" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="D15" s="109">
         <f>'Steel and alu prod'!E14</f>
@@ -16187,7 +16177,7 @@
     <row r="16" spans="2:15" s="137" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B16" s="495"/>
       <c r="C16" s="493" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D16" s="109">
         <f>'Steel and alu prod'!E15</f>
@@ -16284,7 +16274,7 @@
     </row>
     <row r="20" spans="2:15" s="137" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B20" s="660" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C20" s="493"/>
       <c r="D20" s="110"/>
@@ -16303,7 +16293,7 @@
     <row r="21" spans="2:15" s="137" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B21" s="660"/>
       <c r="C21" s="493" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D21" s="109">
         <f>'Steel and alu prod'!E11</f>
@@ -16366,7 +16356,7 @@
     </row>
     <row r="23" spans="2:15" s="137" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B23" s="144" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C23" s="491"/>
       <c r="D23" s="145"/>
@@ -16446,7 +16436,7 @@
     <row r="26" spans="2:15" s="137" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B26" s="140"/>
       <c r="C26" s="493" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D26" s="109">
         <f>'Steel and alu prod'!E11</f>
@@ -17081,7 +17071,7 @@
     <row r="11" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B11" s="442"/>
       <c r="C11" s="447" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D11" s="98">
         <f>share_steel_blast_furnace_bof</f>
@@ -17095,7 +17085,7 @@
     <row r="12" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B12" s="442"/>
       <c r="C12" s="447" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D12" s="98">
         <f>share_steel_cyclone_furnace_bof</f>
@@ -17109,7 +17099,7 @@
     <row r="13" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B13" s="442"/>
       <c r="C13" s="447" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D13" s="98">
         <f>share_steel_scrap_hbi_eaf</f>
@@ -17123,7 +17113,7 @@
     <row r="14" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B14" s="442"/>
       <c r="C14" s="447" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="D14" s="98">
         <f>share_steel_dri_network_gas_eaf</f>
@@ -17137,7 +17127,7 @@
     <row r="15" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B15" s="442"/>
       <c r="C15" s="447" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D15" s="98">
         <f>share_steel_dri_hydrogen_eaf</f>
@@ -17415,7 +17405,7 @@
       </c>
       <c r="L10" s="106"/>
       <c r="M10" s="678" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="N10" s="106"/>
       <c r="O10" s="106"/>
@@ -17424,7 +17414,7 @@
       <c r="R10" s="106"/>
       <c r="S10" s="106"/>
       <c r="T10" s="680" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="U10" s="117" t="s">
         <v>459</v>
@@ -17542,7 +17532,7 @@
     <row r="13" spans="2:26" ht="17" x14ac:dyDescent="0.2">
       <c r="B13" s="442"/>
       <c r="C13" s="447" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D13" s="226">
         <f>IFERROR('Steel and alu demand'!G12/'Steel and alu demand'!$F$12,0.056)</f>
@@ -17637,7 +17627,7 @@
     <row r="14" spans="2:26" ht="17" x14ac:dyDescent="0.2">
       <c r="B14" s="442"/>
       <c r="C14" s="447" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D14" s="226">
         <f>IFERROR('Steel and alu demand'!G14/'Steel and alu demand'!$F$14,1-G14-J14)</f>
@@ -18105,7 +18095,7 @@
     </row>
     <row r="11" spans="2:15" s="222" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B11" s="494" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C11" s="497"/>
       <c r="D11" s="319"/>
@@ -18187,7 +18177,7 @@
     </row>
     <row r="14" spans="2:15" s="137" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B14" s="144" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C14" s="491"/>
       <c r="D14" s="328"/>
@@ -18516,7 +18506,7 @@
       <c r="B8" s="93"/>
       <c r="C8" s="455"/>
       <c r="D8" s="106" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="E8" s="106"/>
       <c r="F8" s="106"/>
@@ -18525,7 +18515,7 @@
       <c r="I8" s="106"/>
       <c r="J8" s="106"/>
       <c r="K8" s="678" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="L8" s="117" t="s">
         <v>459</v>
@@ -19131,7 +19121,7 @@
         <v>41534</v>
       </c>
       <c r="C43" s="189" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D43" s="211">
         <v>1.37</v>
@@ -19219,7 +19209,7 @@
         <v>41618</v>
       </c>
       <c r="C51" s="189" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D51" s="211">
         <v>1.43</v>
@@ -19230,7 +19220,7 @@
         <v>41689</v>
       </c>
       <c r="C52" s="189" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D52" s="211">
         <v>1.44</v>
@@ -19241,7 +19231,7 @@
         <v>41690</v>
       </c>
       <c r="C53" s="189" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D53" s="211">
         <v>1.45</v>
@@ -19252,7 +19242,7 @@
         <v>41695</v>
       </c>
       <c r="C54" s="189" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D54" s="211">
         <v>1.46</v>
@@ -19260,10 +19250,10 @@
     </row>
     <row r="55" spans="2:4" ht="153" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="187" t="s">
+        <v>546</v>
+      </c>
+      <c r="C55" s="189" t="s">
         <v>547</v>
-      </c>
-      <c r="C55" s="189" t="s">
-        <v>548</v>
       </c>
       <c r="D55" s="211">
         <v>1.47</v>
@@ -19274,7 +19264,7 @@
         <v>44369</v>
       </c>
       <c r="C56" s="189" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D56" s="211">
         <v>1.48</v>
@@ -19812,7 +19802,7 @@
     </row>
     <row r="22" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="B22" s="146" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C22" s="266"/>
       <c r="D22" s="354">
@@ -20039,7 +20029,7 @@
     <row r="11" spans="2:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B11" s="234"/>
       <c r="C11" s="675" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D11" s="243"/>
       <c r="E11" s="676" t="s">
@@ -20074,7 +20064,7 @@
     <row r="12" spans="2:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B12" s="234"/>
       <c r="C12" s="675" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D12" s="243"/>
       <c r="E12" s="676" t="s">
@@ -21065,7 +21055,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="221" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B3" s="498">
         <f>IFERROR('Shares per carrier per sector'!E11,0)</f>
@@ -21074,7 +21064,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B4" s="498">
         <f>IFERROR('Shares per carrier per sector'!E12,)</f>
@@ -21083,7 +21073,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B5" s="498">
         <f>1-B4-B3</f>
@@ -21141,7 +21131,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -21154,7 +21144,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="221" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B3" s="498">
         <f>IFERROR('Shares per carrier per sector'!E19,0)</f>
@@ -21163,7 +21153,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B4" s="498">
         <f>1-B3</f>
@@ -21211,7 +21201,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="221" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B3" s="498">
         <f>IFERROR('Shares per carrier per sector'!E26,0)</f>
@@ -21220,7 +21210,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B4" s="498">
         <f>IFERROR('Shares per carrier per sector'!E27,0)</f>
@@ -21229,7 +21219,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B5" s="498">
         <f>1-B4-B3</f>
@@ -21267,7 +21257,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -21280,7 +21270,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="221" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B3" s="498">
         <f>IFERROR('Shares per carrier per sector'!E34,0)</f>
@@ -21289,7 +21279,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B4" s="498">
         <f>1-B3</f>
@@ -21338,7 +21328,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="221" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B3" s="498">
         <f>IFERROR('Shares per carrier per sector'!E38,0)</f>
@@ -21347,7 +21337,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B4" s="498">
         <f>1-B3</f>
@@ -21384,7 +21374,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -21397,7 +21387,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="221" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B3" s="499">
         <f>1-B4</f>
@@ -21406,7 +21396,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B4" s="499">
         <f>IFERROR('Shares per carrier steel'!E13,0)</f>
@@ -21464,7 +21454,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -21477,7 +21467,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="221" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B3" s="499">
         <f>IFERROR('Shares per carrier steel'!E22,1)</f>
@@ -21486,7 +21476,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B4" s="499">
         <f>IFERROR('Shares per carrier steel'!E24, 0)</f>
@@ -21651,7 +21641,7 @@
         <v>271</v>
       </c>
       <c r="C17" s="272" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="18" spans="2:3" s="81" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
@@ -21768,50 +21758,50 @@
     </row>
     <row r="32" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="136" t="s">
+        <v>528</v>
+      </c>
+      <c r="C32" s="269" t="s">
         <v>529</v>
-      </c>
-      <c r="C32" s="269" t="s">
-        <v>530</v>
       </c>
     </row>
     <row r="33" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="136" t="s">
+        <v>530</v>
+      </c>
+      <c r="C33" s="269" t="s">
         <v>531</v>
-      </c>
-      <c r="C33" s="269" t="s">
-        <v>532</v>
       </c>
     </row>
     <row r="34" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="136" t="s">
+        <v>532</v>
+      </c>
+      <c r="C34" s="269" t="s">
         <v>533</v>
-      </c>
-      <c r="C34" s="269" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="35" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="136" t="s">
+        <v>534</v>
+      </c>
+      <c r="C35" s="269" t="s">
         <v>535</v>
-      </c>
-      <c r="C35" s="269" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="36" spans="2:3" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="275" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C36" s="276" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="37" spans="2:3" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="275" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C37" s="276" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="38" spans="2:3" ht="28" customHeight="1" x14ac:dyDescent="0.2">
@@ -21819,7 +21809,7 @@
         <v>494</v>
       </c>
       <c r="C38" s="276" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
   </sheetData>
@@ -21852,7 +21842,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -21865,7 +21855,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="221" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B3" s="499">
         <f>1-B4</f>
@@ -21874,7 +21864,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B4" s="499">
         <f>IFERROR('Shares per carrier steel'!E37,0)</f>
@@ -21929,7 +21919,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="221" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -22103,7 +22093,7 @@
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -22182,7 +22172,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -22197,7 +22187,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B3" s="498">
         <f>'Shares coal gas distribution'!E18</f>
@@ -22207,7 +22197,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B4" s="498">
         <f>'Shares coal gas distribution'!E17</f>
@@ -22216,7 +22206,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B5" s="498">
         <f>1-SUM(B3:B4)</f>
@@ -22250,7 +22240,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -22265,7 +22255,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="B3" s="498">
         <f>'Shares coal gas distribution'!E12</f>
@@ -22275,7 +22265,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B4" s="498">
         <f>1-B3</f>
@@ -22316,7 +22306,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="221" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -22365,7 +22355,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="661" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B7" s="181">
         <f>'Steel and alu eff'!G13</f>
@@ -22374,7 +22364,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="661" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B8" s="181">
         <f>'Steel and alu eff'!H13</f>
@@ -22383,7 +22373,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="661" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B9" s="181">
         <f>'Steel and alu eff'!I13</f>
@@ -22437,7 +22427,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="221" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -22468,7 +22458,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="661" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B5" s="181">
         <f>'Steel and alu eff'!G14</f>
@@ -22525,7 +22515,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="221" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -22538,7 +22528,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="661" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="B3" s="181" t="e">
         <f>'Shares per carrier aluminium'!E11</f>
@@ -22547,7 +22537,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="661" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="B4" s="181" t="e">
         <f>'Shares per carrier aluminium'!E12</f>
@@ -22556,7 +22546,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="661" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="B5" s="181" t="e">
         <f>'Shares per carrier aluminium'!E13</f>
@@ -22565,7 +22555,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="661" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="B6" s="181" t="e">
         <f>'Shares per carrier aluminium'!E14</f>
@@ -22608,7 +22598,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -22621,7 +22611,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="661" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="B3" s="181" t="e">
         <f>'Shares per carrier aluminium'!E17</f>
@@ -22630,7 +22620,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="661" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="B4" s="181" t="e">
         <f>'Shares per carrier aluminium'!E18</f>
@@ -22639,7 +22629,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="661" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="B5" s="181" t="e">
         <f>'Shares per carrier aluminium'!E19</f>
@@ -22648,7 +22638,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="661" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="B6" s="181" t="e">
         <f>'Shares per carrier aluminium'!E20</f>
@@ -22681,7 +22671,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="221" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -22703,7 +22693,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="661" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B4" s="181">
         <f>IFERROR('Final demand'!G21/SUM('Final demand'!C21,'Final demand'!F21,'Final demand'!G21),0)</f>
@@ -22712,7 +22702,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="661" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B5" s="181">
         <f>1-B4-B3</f>
@@ -22866,7 +22856,7 @@
   <sheetData>
     <row r="2" spans="2:80" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="55" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C2" s="52"/>
       <c r="D2" s="52"/>
@@ -23507,7 +23497,7 @@
     <row r="28" spans="2:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B28" s="606"/>
       <c r="C28" s="602" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D28" s="609" t="s">
         <v>298</v>
@@ -24175,7 +24165,7 @@
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B5" s="695" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C5" s="696"/>
       <c r="D5" s="696"/>
@@ -24307,7 +24297,7 @@
       </c>
       <c r="D13" s="284"/>
       <c r="E13" s="290" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="F13" s="290"/>
       <c r="G13" s="19" t="s">
@@ -24450,7 +24440,7 @@
     <row r="19" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="27"/>
       <c r="C19" s="401" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D19" s="285"/>
       <c r="E19" s="292">
@@ -24459,7 +24449,7 @@
       </c>
       <c r="F19" s="283"/>
       <c r="G19" s="405" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="H19" s="8"/>
       <c r="I19" s="20"/>
@@ -24476,7 +24466,7 @@
       </c>
       <c r="N19" s="8"/>
       <c r="O19" s="410" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="P19" s="7">
         <f>IF(L19=TRUE,1,0)</f>
@@ -24486,7 +24476,7 @@
     <row r="20" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="27"/>
       <c r="C20" s="401" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D20" s="285"/>
       <c r="E20" s="292">
@@ -24494,7 +24484,7 @@
       </c>
       <c r="F20" s="283"/>
       <c r="G20" s="405" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
@@ -24504,20 +24494,20 @@
       <c r="M20" s="28"/>
       <c r="N20" s="8"/>
       <c r="O20" s="410" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="P20" s="411"/>
     </row>
     <row r="21" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B21" s="27"/>
       <c r="C21" s="401" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D21" s="285"/>
       <c r="E21" s="662"/>
       <c r="F21" s="283"/>
       <c r="G21" s="405" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="H21" s="8"/>
       <c r="I21" s="20"/>
@@ -24527,14 +24517,14 @@
       <c r="M21" s="560"/>
       <c r="N21" s="289"/>
       <c r="O21" s="410" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="P21" s="411"/>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B22" s="27"/>
       <c r="C22" s="401" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D22" s="285"/>
       <c r="E22" s="292">
@@ -24542,7 +24532,7 @@
       </c>
       <c r="F22" s="283"/>
       <c r="G22" s="405" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
@@ -24552,14 +24542,14 @@
       <c r="M22" s="560"/>
       <c r="N22" s="289"/>
       <c r="O22" s="410" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="P22" s="411"/>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B23" s="27"/>
       <c r="C23" s="401" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D23" s="285"/>
       <c r="E23" s="292">
@@ -24567,7 +24557,7 @@
       </c>
       <c r="F23" s="283"/>
       <c r="G23" s="405" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
@@ -24577,7 +24567,7 @@
       <c r="M23" s="559"/>
       <c r="N23" s="8"/>
       <c r="O23" s="410" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="P23" s="411"/>
     </row>
@@ -24616,13 +24606,13 @@
     <row r="26" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="32"/>
       <c r="C26" s="8" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="D26" s="285"/>
       <c r="E26" s="664"/>
       <c r="F26" s="283"/>
       <c r="G26" s="405" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="H26" s="8"/>
       <c r="I26" s="20"/>
@@ -24640,7 +24630,7 @@
       </c>
       <c r="N26" s="8"/>
       <c r="O26" s="410" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="P26" s="7">
         <f>IF(L26=TRUE,1,0)</f>
@@ -24650,7 +24640,7 @@
     <row r="27" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B27" s="32"/>
       <c r="C27" s="8" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D27" s="285"/>
       <c r="E27" s="666">
@@ -24659,7 +24649,7 @@
       </c>
       <c r="F27" s="283"/>
       <c r="G27" s="405" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="H27" s="8"/>
       <c r="I27" s="8"/>
@@ -24691,13 +24681,13 @@
     <row r="29" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B29" s="27"/>
       <c r="C29" s="8" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D29" s="285"/>
       <c r="E29" s="664"/>
       <c r="F29" s="398"/>
       <c r="G29" s="405" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="H29" s="8"/>
       <c r="I29" s="20"/>
@@ -24712,7 +24702,7 @@
       <c r="M29" s="558"/>
       <c r="N29" s="8"/>
       <c r="O29" s="410" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="P29" s="7">
         <v>1</v>
@@ -24721,7 +24711,7 @@
     <row r="30" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B30" s="27"/>
       <c r="C30" s="8" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D30" s="285"/>
       <c r="E30" s="666">
@@ -24730,7 +24720,7 @@
       </c>
       <c r="F30" s="398"/>
       <c r="G30" s="405" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="H30" s="8"/>
       <c r="I30" s="8"/>
@@ -24762,13 +24752,13 @@
     <row r="32" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B32" s="27"/>
       <c r="C32" s="8" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="D32" s="285"/>
       <c r="E32" s="667"/>
       <c r="F32" s="283"/>
       <c r="G32" s="405" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="H32" s="8"/>
       <c r="I32" s="20"/>
@@ -24783,7 +24773,7 @@
       <c r="M32" s="559"/>
       <c r="N32" s="8"/>
       <c r="O32" s="410" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="P32" s="411">
         <v>1</v>
@@ -24792,7 +24782,7 @@
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B33" s="27"/>
       <c r="C33" s="8" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D33" s="285"/>
       <c r="E33" s="665">
@@ -24801,7 +24791,7 @@
       </c>
       <c r="F33" s="283"/>
       <c r="G33" s="405" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="H33" s="8"/>
       <c r="I33" s="8"/>
@@ -24832,7 +24822,7 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B35" s="32" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C35" s="401"/>
       <c r="D35" s="285"/>
@@ -24869,10 +24859,10 @@
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B37" s="32"/>
       <c r="C37" s="401" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D37" s="285" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="E37" s="206" t="e">
         <f>'Steel and alu demand'!E12</f>
@@ -24893,10 +24883,10 @@
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B38" s="32"/>
       <c r="C38" s="401" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="D38" s="285" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="E38" s="206" t="e">
         <f>'Steel and alu demand'!E14</f>
@@ -24954,7 +24944,7 @@
       <c r="A41" s="8"/>
       <c r="B41" s="32"/>
       <c r="C41" s="8" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D41" s="285" t="s">
         <v>324</v>
@@ -25011,7 +25001,7 @@
       <c r="A43" s="8"/>
       <c r="B43" s="27"/>
       <c r="C43" s="8" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D43" s="285" t="s">
         <v>324</v>
@@ -25069,7 +25059,7 @@
       <c r="A45" s="8"/>
       <c r="B45" s="27"/>
       <c r="C45" s="8" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D45" s="285" t="s">
         <v>324</v>
@@ -25127,7 +25117,7 @@
       <c r="A47" s="8"/>
       <c r="B47" s="27"/>
       <c r="C47" s="8" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D47" s="285" t="s">
         <v>324</v>
@@ -25185,7 +25175,7 @@
       <c r="A49" s="8"/>
       <c r="B49" s="27"/>
       <c r="C49" s="8" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D49" s="285" t="s">
         <v>324</v>
@@ -25425,7 +25415,7 @@
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B59" s="32" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C59" s="8"/>
       <c r="D59" s="285"/>
@@ -32745,7 +32735,7 @@
   </sheetPr>
   <dimension ref="B2:S77"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
@@ -32784,7 +32774,7 @@
     </row>
     <row r="5" spans="2:19" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="701" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C5" s="702"/>
       <c r="D5" s="702"/>
@@ -32824,7 +32814,7 @@
       <c r="P7" s="524"/>
       <c r="Q7" s="524"/>
       <c r="R7" s="569" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="S7" s="527" t="s">
         <v>489</v>
@@ -32890,7 +32880,7 @@
         <v>407</v>
       </c>
       <c r="P9" s="533" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="Q9" s="582" t="s">
         <v>485</v>
@@ -32942,7 +32932,7 @@
     </row>
     <row r="12" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="89" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C12" s="90" t="s">
         <v>231</v>
@@ -33179,7 +33169,7 @@
         <v>231</v>
       </c>
       <c r="C22" s="421" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D22" s="425" t="s">
         <v>404</v>
@@ -33202,7 +33192,7 @@
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B23" s="36" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C23" s="92"/>
       <c r="D23" s="508"/>
@@ -33225,12 +33215,10 @@
     <row r="24" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B24" s="36"/>
       <c r="C24" s="418" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D24" s="374"/>
-      <c r="E24" s="418" t="s">
-        <v>641</v>
-      </c>
+      <c r="E24" s="418"/>
       <c r="F24" s="418"/>
       <c r="G24" s="418"/>
       <c r="H24" s="418"/>
@@ -33249,7 +33237,7 @@
     <row r="25" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B25" s="36"/>
       <c r="C25" s="577" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D25" s="553" t="e">
         <f t="shared" ref="D25:D26" si="0">S25</f>
@@ -33279,7 +33267,7 @@
     <row r="26" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B26" s="36"/>
       <c r="C26" s="577" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D26" s="553" t="e">
         <f t="shared" si="0"/>
@@ -33309,7 +33297,7 @@
     <row r="27" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B27" s="36"/>
       <c r="C27" s="577" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D27" s="553" t="e">
         <f>S27</f>
@@ -33339,7 +33327,7 @@
     <row r="28" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B28" s="36"/>
       <c r="C28" s="577" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D28" s="553" t="e">
         <f t="shared" ref="D28:D30" si="1">S28</f>
@@ -33369,7 +33357,7 @@
     <row r="29" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B29" s="36"/>
       <c r="C29" s="577" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D29" s="553" t="e">
         <f t="shared" si="1"/>
@@ -33462,9 +33450,7 @@
         <v>208</v>
       </c>
       <c r="D32" s="509"/>
-      <c r="E32" s="528" t="s">
-        <v>644</v>
-      </c>
+      <c r="E32" s="528"/>
       <c r="F32" s="418"/>
       <c r="G32" s="418"/>
       <c r="H32" s="418"/>
@@ -33483,7 +33469,7 @@
     <row r="33" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B33" s="36"/>
       <c r="C33" s="577" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D33" s="509" t="e">
         <f>S33</f>
@@ -33513,7 +33499,7 @@
     <row r="34" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B34" s="36"/>
       <c r="C34" s="577" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D34" s="509" t="e">
         <f>S34</f>
@@ -33543,7 +33529,7 @@
     <row r="35" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B35" s="36"/>
       <c r="C35" s="577" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D35" s="509" t="e">
         <f>S35</f>
@@ -33667,7 +33653,7 @@
         <v>231</v>
       </c>
       <c r="C40" s="421" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D40" s="427" t="s">
         <v>452</v>
@@ -33713,12 +33699,10 @@
     <row r="42" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B42" s="36"/>
       <c r="C42" s="418" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D42" s="652"/>
-      <c r="E42" s="418" t="s">
-        <v>642</v>
-      </c>
+      <c r="E42" s="418"/>
       <c r="F42" s="418"/>
       <c r="G42" s="418"/>
       <c r="H42" s="418"/>
@@ -33737,7 +33721,7 @@
     <row r="43" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B43" s="36"/>
       <c r="C43" s="577" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D43" s="553" t="e">
         <f t="shared" ref="D43:D44" si="2">S43</f>
@@ -33767,7 +33751,7 @@
     <row r="44" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B44" s="36"/>
       <c r="C44" s="577" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D44" s="553" t="e">
         <f t="shared" si="2"/>
@@ -33797,7 +33781,7 @@
     <row r="45" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B45" s="93"/>
       <c r="C45" s="577" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D45" s="553" t="e">
         <f>S45</f>
@@ -33827,7 +33811,7 @@
     <row r="46" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B46" s="93"/>
       <c r="C46" s="577" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D46" s="553" t="e">
         <f t="shared" ref="D46:D48" si="3">S46</f>
@@ -33857,7 +33841,7 @@
     <row r="47" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B47" s="93"/>
       <c r="C47" s="577" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D47" s="553" t="e">
         <f t="shared" si="3"/>
@@ -33950,9 +33934,7 @@
         <v>208</v>
       </c>
       <c r="D50" s="553"/>
-      <c r="E50" s="418" t="s">
-        <v>503</v>
-      </c>
+      <c r="E50" s="418"/>
       <c r="F50" s="418"/>
       <c r="G50" s="418"/>
       <c r="H50" s="418"/>
@@ -33971,7 +33953,7 @@
     <row r="51" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B51" s="93"/>
       <c r="C51" s="577" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D51" s="553" t="e">
         <f>S51</f>
@@ -34001,7 +33983,7 @@
     <row r="52" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B52" s="93"/>
       <c r="C52" s="577" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D52" s="553" t="e">
         <f>S52</f>
@@ -34031,7 +34013,7 @@
     <row r="53" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B53" s="93"/>
       <c r="C53" s="577" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D53" s="553" t="e">
         <f>S53</f>
@@ -34125,7 +34107,7 @@
         <v>231</v>
       </c>
       <c r="C57" s="421" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D57" s="511" t="s">
         <v>404</v>
@@ -34175,7 +34157,7 @@
       </c>
       <c r="D59" s="585"/>
       <c r="E59" s="528" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F59" s="418"/>
       <c r="G59" s="418"/>
@@ -34301,7 +34283,7 @@
       </c>
       <c r="D64" s="585"/>
       <c r="E64" s="528" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F64" s="418"/>
       <c r="G64" s="418"/>
@@ -34427,7 +34409,7 @@
       </c>
       <c r="D69" s="585"/>
       <c r="E69" s="528" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F69" s="418"/>
       <c r="G69" s="418"/>
@@ -34553,7 +34535,7 @@
       </c>
       <c r="D74" s="585"/>
       <c r="E74" s="528" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F74" s="418"/>
       <c r="G74" s="418"/>

</xml_diff>